<commit_message>
El que faltaba :D
</commit_message>
<xml_diff>
--- a/Proyecto/Escritorio/Metáforas/Índice de interfaces.xlsx
+++ b/Proyecto/Escritorio/Metáforas/Índice de interfaces.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coner\Dropbox\Proyectos\Proyecto\Escritorio\Metáforas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151C3652-403A-4CBC-926F-E8455840A592}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61798159-4F93-4422-899A-61B6C99557C8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3135" yWindow="390" windowWidth="11745" windowHeight="8340" xr2:uid="{DCB1A162-0AA3-4A80-BDB3-140FF87E20A2}"/>
   </bookViews>
@@ -20,17 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
   <si>
     <t>Módulo</t>
   </si>
@@ -47,9 +42,6 @@
     <t>módulosAcceso // menuPrincipal</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>iC</t>
   </si>
   <si>
@@ -210,6 +202,18 @@
   </si>
   <si>
     <t>(más claro)</t>
+  </si>
+  <si>
+    <t>Resolución de imágenes</t>
+  </si>
+  <si>
+    <t>[144, 144]</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>mA</t>
   </si>
 </sst>
 </file>
@@ -570,13 +574,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D96A41-003B-455E-85B5-CC96546B3570}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -584,9 +589,11 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
@@ -602,7 +609,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -613,278 +620,302 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>48</v>
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>48</v>
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>61</v>
       </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
         <v>53</v>
-      </c>
-      <c r="C28" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" t="s">
         <v>58</v>
-      </c>
-      <c r="C32" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>